<commit_message>
AutoCommit_10 октября 2023 г. 8:24:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>2ОИБАС1022: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Инд1</t>
+  </si>
+  <si>
+    <t>Лаб1</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -527,7 +530,9 @@
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -565,7 +570,9 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -756,7 +763,9 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_10 октября 2023 г. 8:29:35_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -491,7 +491,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,9 @@
       <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_10 октября 2023 г. 8:52:07_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -491,7 +491,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -664,7 +664,9 @@
       <c r="C12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -736,7 +738,9 @@
         <v>13</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_10 октября 2023 г. 9:03:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -488,10 +488,10 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -772,7 +772,9 @@
       <c r="C19" s="2">
         <v>5</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -834,7 +836,9 @@
       <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -906,7 +910,9 @@
       <c r="C28" s="2">
         <v>5</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 11:25:16_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ОИБАС1022: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>Лаб1</t>
+  </si>
+  <si>
+    <t>Лаб2</t>
+  </si>
+  <si>
+    <t>Лаб3</t>
+  </si>
+  <si>
+    <t>Лаб4</t>
+  </si>
+  <si>
+    <t>Лаб5</t>
+  </si>
+  <si>
+    <t>Инд2</t>
+  </si>
+  <si>
+    <t>Инд3</t>
+  </si>
+  <si>
+    <t>Инд4</t>
+  </si>
+  <si>
+    <t>Инд5</t>
   </si>
 </sst>
 </file>
@@ -185,11 +209,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -497,10 +521,10 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C29" activeCellId="4" sqref="D19 D23 D28 C27 C29"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -511,51 +535,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-    </row>
-    <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -563,31 +608,31 @@
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -595,13 +640,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -609,47 +654,50 @@
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6">
-        <v>5</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -657,31 +705,34 @@
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6">
-        <v>5</v>
-      </c>
-      <c r="D12" s="6">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -689,29 +740,32 @@
         <v>9</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="6">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -719,13 +773,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -733,13 +787,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -747,49 +801,49 @@
         <v>13</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="6">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="H17" s="4">
+        <v>5</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="6">
-        <v>5</v>
-      </c>
-      <c r="D19" s="6">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4">
+        <v>5</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -797,63 +851,63 @@
         <v>16</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="6">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="6">
-        <v>5</v>
-      </c>
-      <c r="D23" s="6">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -861,13 +915,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -875,13 +929,13 @@
         <v>21</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -889,27 +943,27 @@
         <v>22</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="C27" s="4"/>
       <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -919,37 +973,37 @@
       <c r="C28" s="2">
         <v>5</v>
       </c>
-      <c r="D28" s="6">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="H28" s="4">
+        <v>5</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="6">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="C29" s="4">
+        <v>5</v>
+      </c>
       <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
       <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 13:02:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -215,11 +215,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -527,10 +527,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -541,29 +541,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -730,6 +730,9 @@
       <c r="E12">
         <v>5</v>
       </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
       <c r="H12" s="4">
         <v>5</v>
       </c>
@@ -935,6 +938,12 @@
         <v>21</v>
       </c>
       <c r="C25" s="2"/>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1012,7 +1021,7 @@
       <c r="L30" s="3"/>
     </row>
     <row r="32" spans="1:12" ht="13" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F32">

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 14:18:03_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -527,10 +527,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -738,7 +738,9 @@
       <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -771,7 +773,9 @@
         <v>3</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -833,7 +837,9 @@
       <c r="H18" s="2">
         <v>5</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="2">
+        <v>5</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -948,8 +954,12 @@
       <c r="G25">
         <v>5</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="H25" s="2">
+        <v>5</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4</v>
+      </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 14:19:15_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -527,10 +527,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,9 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="L28" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1024,7 +1026,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="L29" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 17:30:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -218,8 +218,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -526,11 +528,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -541,29 +543,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -619,6 +621,13 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
+      <c r="N5">
+        <f>SUM(C5:L5)</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -637,6 +646,13 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
+      <c r="N6" s="6">
+        <f t="shared" ref="N6:N29" si="0">SUM(C6:L6)</f>
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -651,6 +667,13 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
+      <c r="N7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -665,6 +688,13 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
+      <c r="N8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -676,13 +706,20 @@
       <c r="C9" s="4">
         <v>5</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="4">
         <v>5</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
+      <c r="N9" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -694,7 +731,7 @@
       <c r="C10" s="4">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="9">
         <v>5</v>
       </c>
       <c r="H10" s="4">
@@ -704,6 +741,13 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
+      <c r="N10" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -718,6 +762,13 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
+      <c r="N11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -729,21 +780,28 @@
       <c r="C12" s="4">
         <v>5</v>
       </c>
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="9">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9">
         <v>5</v>
       </c>
       <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="4">
         <v>3</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
+      <c r="N12" s="6">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -758,6 +816,13 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
+      <c r="N13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -769,16 +834,23 @@
       <c r="C14" s="4">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="9">
         <v>3</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="2">
+      <c r="I14" s="4">
         <v>5</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
+      <c r="N14" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -793,6 +865,13 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
+      <c r="N15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -807,8 +886,15 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -823,8 +909,15 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -834,17 +927,24 @@
       <c r="C18" s="4">
         <v>5</v>
       </c>
-      <c r="H18" s="2">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2">
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
         <v>5</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -861,8 +961,15 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -875,8 +982,15 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -891,8 +1005,15 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -907,8 +1028,15 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -925,8 +1053,15 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -939,8 +1074,15 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -948,23 +1090,30 @@
         <v>21</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>5</v>
-      </c>
-      <c r="I25" s="2">
+      <c r="F25" s="9">
+        <v>5</v>
+      </c>
+      <c r="G25" s="9">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4">
+        <v>5</v>
+      </c>
+      <c r="I25" s="4">
         <v>4</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -977,8 +1126,15 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -991,15 +1147,22 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <v>5</v>
       </c>
       <c r="H28" s="4">
@@ -1011,8 +1174,15 @@
       <c r="L28" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1029,8 +1199,15 @@
       <c r="L29" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N29" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1038,7 +1215,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>36</v>
       </c>
@@ -1051,6 +1228,30 @@
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
+  <conditionalFormatting sqref="N5:N29">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:P29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 12:05:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -226,11 +226,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -538,10 +538,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -552,29 +552,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -645,7 +645,7 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>5</v>
       </c>
       <c r="H6" s="4">
@@ -936,6 +936,9 @@
       <c r="C18" s="4">
         <v>5</v>
       </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
       <c r="H18" s="4">
         <v>5</v>
       </c>
@@ -947,7 +950,7 @@
       <c r="L18" s="2"/>
       <c r="N18" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P18">
         <v>5</v>
@@ -1227,6 +1230,9 @@
     <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
       </c>
       <c r="F32">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 13:46:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -538,10 +538,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -648,6 +648,12 @@
       <c r="C6" s="8">
         <v>5</v>
       </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
       <c r="H6" s="4">
         <v>5</v>
       </c>
@@ -657,7 +663,7 @@
       <c r="L6" s="2"/>
       <c r="N6" s="6">
         <f t="shared" ref="N6:N29" si="0">SUM(C6:L6)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P6">
         <v>4</v>
@@ -846,6 +852,9 @@
       <c r="E14" s="7">
         <v>3</v>
       </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="4">
         <v>5</v>
@@ -855,7 +864,7 @@
       <c r="L14" s="2"/>
       <c r="N14" s="6">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="P14">
         <v>5</v>
@@ -939,6 +948,9 @@
       <c r="D18">
         <v>5</v>
       </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
       <c r="H18" s="4">
         <v>5</v>
       </c>
@@ -950,7 +962,7 @@
       <c r="L18" s="2"/>
       <c r="N18" s="6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="P18">
         <v>5</v>
@@ -1012,6 +1024,9 @@
       <c r="C21" s="4">
         <v>5</v>
       </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1019,7 +1034,7 @@
       <c r="L21" s="2"/>
       <c r="N21" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 13:54:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -541,7 +541,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -951,6 +951,9 @@
       <c r="F18">
         <v>5</v>
       </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
       <c r="H18" s="4">
         <v>5</v>
       </c>
@@ -962,7 +965,7 @@
       <c r="L18" s="2"/>
       <c r="N18" s="6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="P18">
         <v>5</v>
@@ -1027,14 +1030,16 @@
       <c r="F21">
         <v>5</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>5</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="N21" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 14:06:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -541,7 +541,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -657,13 +657,15 @@
       <c r="H6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="N6" s="6">
         <f t="shared" ref="N6:N29" si="0">SUM(C6:L6)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="P6">
         <v>4</v>
@@ -1033,13 +1035,15 @@
       <c r="H21" s="2">
         <v>5</v>
       </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="N21" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 14:07:13_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -541,7 +541,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -660,12 +660,16 @@
       <c r="I6" s="2">
         <v>5</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>5</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="N6" s="6">
         <f t="shared" ref="N6:N29" si="0">SUM(C6:L6)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P6">
         <v>4</v>
@@ -962,12 +966,16 @@
       <c r="I18" s="4">
         <v>5</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>5</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="N18" s="6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="P18">
         <v>5</v>
@@ -1040,10 +1048,12 @@
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2">
+        <v>4</v>
+      </c>
       <c r="N21" s="6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="P21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_17 ноября 2023 г. 22:39:39_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -226,12 +226,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -539,10 +539,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -553,29 +553,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -646,25 +646,25 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10">
-        <v>5</v>
-      </c>
-      <c r="F6" s="11">
-        <v>5</v>
-      </c>
-      <c r="G6">
+      <c r="C6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="9">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7">
         <v>5</v>
       </c>
       <c r="H6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="2">
-        <v>5</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
+      <c r="K6" s="4">
         <v>5</v>
       </c>
       <c r="L6" s="2"/>
@@ -859,7 +859,7 @@
       <c r="E14" s="7">
         <v>3</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>5</v>
       </c>
       <c r="H14" s="2"/>
@@ -952,13 +952,13 @@
       <c r="C18" s="4">
         <v>5</v>
       </c>
-      <c r="D18" s="11">
-        <v>5</v>
-      </c>
-      <c r="F18" s="11">
-        <v>5</v>
-      </c>
-      <c r="G18">
+      <c r="D18" s="9">
+        <v>5</v>
+      </c>
+      <c r="F18" s="9">
+        <v>5</v>
+      </c>
+      <c r="G18" s="7">
         <v>5</v>
       </c>
       <c r="H18" s="4">
@@ -967,10 +967,10 @@
       <c r="I18" s="4">
         <v>5</v>
       </c>
-      <c r="J18" s="2">
-        <v>5</v>
-      </c>
-      <c r="K18" s="2">
+      <c r="J18" s="4">
+        <v>5</v>
+      </c>
+      <c r="K18" s="4">
         <v>5</v>
       </c>
       <c r="L18" s="2"/>
@@ -1038,18 +1038,18 @@
       <c r="C21" s="4">
         <v>5</v>
       </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2">
-        <v>5</v>
-      </c>
-      <c r="I21" s="2">
+      <c r="F21" s="7">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4">
         <v>5</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2">
+      <c r="L21" s="4">
         <v>4</v>
       </c>
       <c r="N21" s="6">
@@ -1218,7 +1218,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2">
+      <c r="L28" s="4">
         <v>4</v>
       </c>
       <c r="N28" s="6">
@@ -1243,7 +1243,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="2">
+      <c r="L29" s="4">
         <v>4</v>
       </c>
       <c r="N29" s="6">

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 20:52:24_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -631,13 +631,6 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="N5">
-        <f>SUM(C5:L5)</f>
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -668,13 +661,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="N6" s="6">
-        <f t="shared" ref="N6:N29" si="0">SUM(C6:L6)</f>
-        <v>35</v>
-      </c>
-      <c r="P6">
-        <v>4</v>
-      </c>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -689,13 +676,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="N7" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>2</v>
-      </c>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -704,19 +685,15 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="N8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>2</v>
-      </c>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -735,13 +712,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="N9" s="6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="P9">
-        <v>4</v>
-      </c>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -763,13 +734,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="N10" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -784,13 +749,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="N11" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>2</v>
-      </c>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -817,13 +776,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="N12" s="6">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="P12">
-        <v>5</v>
-      </c>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -838,13 +791,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="N13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -869,13 +816,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="N14" s="6">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="P14">
-        <v>5</v>
-      </c>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -890,13 +831,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="N15" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>2</v>
-      </c>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -911,15 +846,9 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="N16" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -934,15 +863,9 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="N17" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="P17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -974,15 +897,9 @@
         <v>5</v>
       </c>
       <c r="L18" s="2"/>
-      <c r="N18" s="6">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="P18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -999,15 +916,9 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="N19" s="6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="P19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1020,15 +931,9 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="N20" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1052,15 +957,9 @@
       <c r="L21" s="4">
         <v>4</v>
       </c>
-      <c r="N21" s="6">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="P21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1075,15 +974,9 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="N22" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="P22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1100,15 +993,9 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="N23" s="6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="P23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1121,15 +1008,9 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="N24" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1152,15 +1033,9 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="N25" s="6">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="P25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1173,15 +1048,9 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="N26" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1194,15 +1063,9 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="N27" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1221,15 +1084,9 @@
       <c r="L28" s="4">
         <v>4</v>
       </c>
-      <c r="N28" s="6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="P28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1246,15 +1103,9 @@
       <c r="L29" s="4">
         <v>4</v>
       </c>
-      <c r="N29" s="6">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="P29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1262,7 +1113,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 21:22:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4:P33"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -688,10 +688,30 @@
       <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5</v>
+      </c>
       <c r="L8" s="2"/>
       <c r="N8" s="6"/>
     </row>
@@ -809,7 +829,9 @@
       <c r="F14" s="9">
         <v>5</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
       <c r="I14" s="4">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 0:04:36_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -129,7 +129,7 @@
     <t>Инд5</t>
   </si>
   <si>
-    <t>абдулова таисия</t>
+    <t>Абдулова таисия</t>
   </si>
 </sst>
 </file>
@@ -227,8 +227,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -238,6 +236,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -545,10 +545,10 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -559,29 +559,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E4">
@@ -635,7 +635,7 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
@@ -649,7 +649,7 @@
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7">
@@ -680,7 +680,7 @@
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2"/>
@@ -695,7 +695,7 @@
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2">
@@ -732,7 +732,7 @@
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4">
@@ -751,7 +751,7 @@
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
@@ -760,10 +760,15 @@
       <c r="E10" s="6">
         <v>5</v>
       </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
       <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -773,7 +778,7 @@
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
@@ -788,7 +793,7 @@
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4">
@@ -815,7 +820,7 @@
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="2"/>
@@ -1038,8 +1043,21 @@
         <v>20</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_25 декабря 2023 г. 22:22:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>2ОИБАС1022: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>Авдулова Таисия</t>
+  </si>
+  <si>
+    <t>Инд6</t>
+  </si>
+  <si>
+    <t>Инд7</t>
+  </si>
+  <si>
+    <t>Инд8</t>
+  </si>
+  <si>
+    <t>Инд9</t>
   </si>
 </sst>
 </file>
@@ -531,13 +543,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -548,12 +560,12 @@
     <col min="4" max="13" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -573,22 +585,34 @@
         <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(B3=C3,A2+1,"---")</f>
         <v>1</v>
@@ -605,9 +629,9 @@
       <c r="G3">
         <v>4</v>
       </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A28" si="0">IF(B4=C4,A3+1,"---")</f>
         <v>2</v>
@@ -619,13 +643,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -645,21 +669,21 @@
       <c r="H5" s="5">
         <v>5</v>
       </c>
-      <c r="I5" s="4">
-        <v>5</v>
-      </c>
-      <c r="J5" s="4">
-        <v>5</v>
-      </c>
-      <c r="K5" s="4">
-        <v>5</v>
-      </c>
-      <c r="L5" s="4">
-        <v>5</v>
-      </c>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="4">
+        <v>5</v>
+      </c>
+      <c r="N5" s="4">
+        <v>5</v>
+      </c>
+      <c r="O5" s="4">
+        <v>5</v>
+      </c>
+      <c r="P5" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -671,13 +695,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -703,21 +727,21 @@
       <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="2">
-        <v>5</v>
-      </c>
-      <c r="J7" s="2">
-        <v>5</v>
-      </c>
-      <c r="K7" s="2">
-        <v>5</v>
-      </c>
-      <c r="L7" s="2">
-        <v>5</v>
-      </c>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <v>5</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -731,15 +755,15 @@
       <c r="D8" s="4">
         <v>5</v>
       </c>
-      <c r="I8" s="4">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="4">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -759,17 +783,17 @@
       <c r="G9">
         <v>5</v>
       </c>
-      <c r="I9" s="4">
-        <v>5</v>
-      </c>
-      <c r="J9" s="2">
-        <v>5</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="4">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2">
+        <v>5</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -781,13 +805,13 @@
         <v>7</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -807,17 +831,17 @@
       <c r="G11" s="5">
         <v>5</v>
       </c>
-      <c r="I11" s="4">
-        <v>5</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="M11" s="4">
+        <v>5</v>
+      </c>
+      <c r="N11" s="4">
         <v>3</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -829,13 +853,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -855,17 +879,17 @@
       <c r="G13" s="7">
         <v>5</v>
       </c>
-      <c r="I13" s="2">
-        <v>5</v>
-      </c>
-      <c r="J13" s="4">
-        <v>5</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="4">
+        <v>5</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -877,13 +901,13 @@
         <v>11</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -895,13 +919,13 @@
         <v>12</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -913,15 +937,15 @@
         <v>13</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="I16" s="4">
-        <v>5</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="4">
+        <v>5</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -944,21 +968,21 @@
       <c r="H17" s="5">
         <v>5</v>
       </c>
-      <c r="I17" s="4">
-        <v>5</v>
-      </c>
-      <c r="J17" s="4">
-        <v>5</v>
-      </c>
-      <c r="K17" s="4">
-        <v>5</v>
-      </c>
-      <c r="L17" s="4">
-        <v>5</v>
-      </c>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="4">
+        <v>5</v>
+      </c>
+      <c r="N17" s="4">
+        <v>5</v>
+      </c>
+      <c r="O17" s="4">
+        <v>5</v>
+      </c>
+      <c r="P17" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -972,15 +996,15 @@
       <c r="D18" s="4">
         <v>5</v>
       </c>
-      <c r="I18" s="4">
-        <v>5</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="4">
+        <v>5</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -992,13 +1016,13 @@
         <v>16</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1015,19 +1039,19 @@
       <c r="G20" s="5">
         <v>5</v>
       </c>
-      <c r="I20" s="4">
-        <v>5</v>
-      </c>
-      <c r="J20" s="4">
-        <v>5</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
       <c r="M20" s="4">
+        <v>5</v>
+      </c>
+      <c r="N20" s="4">
+        <v>5</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1041,13 +1065,13 @@
       <c r="D21" s="4">
         <v>5</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1061,15 +1085,15 @@
       <c r="D22" s="4">
         <v>5</v>
       </c>
-      <c r="I22" s="4">
-        <v>5</v>
-      </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="4">
+        <v>5</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1090,17 +1114,17 @@
       <c r="H23">
         <v>5</v>
       </c>
-      <c r="I23" s="2">
-        <v>5</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5</v>
-      </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="2">
+        <v>5</v>
+      </c>
+      <c r="N23" s="2">
+        <v>5</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1118,17 +1142,17 @@
       <c r="H24" s="5">
         <v>5</v>
       </c>
-      <c r="I24" s="4">
-        <v>5</v>
-      </c>
-      <c r="J24" s="4">
+      <c r="M24" s="4">
+        <v>5</v>
+      </c>
+      <c r="N24" s="4">
         <v>4</v>
       </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1140,13 +1164,13 @@
         <v>22</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1158,13 +1182,13 @@
         <v>23</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1178,17 +1202,17 @@
       <c r="D27" s="4">
         <v>5</v>
       </c>
-      <c r="I27" s="4">
-        <v>5</v>
-      </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
       <c r="M27" s="4">
+        <v>5</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1202,26 +1226,26 @@
       <c r="D28" s="4">
         <v>5</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="4">
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="P4:P28">
+  <conditionalFormatting sqref="T4:T28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_28 декабря 2023 г. 12:03:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022_ОпСис_/2ОИБАС1022_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>2ОИБАС1022: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -142,13 +142,19 @@
   </si>
   <si>
     <t>Инд9</t>
+  </si>
+  <si>
+    <t>симма</t>
+  </si>
+  <si>
+    <t>ТкЗима</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -158,11 +164,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -186,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -209,6 +210,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -220,9 +230,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,6 +246,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -543,13 +553,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="U17" sqref="U17:V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -560,12 +570,12 @@
     <col min="4" max="13" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="10" t="s">
+    <row r="1" spans="1:20" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -611,8 +621,14 @@
       <c r="Q2" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(B3=C3,A2+1,"---")</f>
         <v>1</v>
@@ -620,26 +636,33 @@
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
         <v>4</v>
       </c>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="S3">
+        <f>SUM(D3:Q3)</f>
+        <v>9</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
         <f t="shared" ref="A4:A28" si="0">IF(B4=C4,A3+1,"---")</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
@@ -648,50 +671,64 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="S4" s="9">
+        <f t="shared" ref="S4:S37" si="1">SUM(D4:Q4)</f>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>5</v>
-      </c>
-      <c r="G5" s="7">
-        <v>5</v>
-      </c>
-      <c r="H5" s="5">
-        <v>5</v>
-      </c>
-      <c r="M5" s="4">
-        <v>5</v>
-      </c>
-      <c r="N5" s="4">
-        <v>5</v>
-      </c>
-      <c r="O5" s="4">
-        <v>5</v>
-      </c>
-      <c r="P5" s="4">
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>5</v>
+      </c>
+      <c r="N5" s="3">
+        <v>5</v>
+      </c>
+      <c r="O5" s="3">
+        <v>5</v>
+      </c>
+      <c r="P5" s="3">
         <v>5</v>
       </c>
       <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="S5" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="T5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
@@ -700,108 +737,136 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="S6" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="M7" s="2">
-        <v>5</v>
-      </c>
-      <c r="N7" s="2">
-        <v>5</v>
-      </c>
-      <c r="O7" s="2">
-        <v>5</v>
-      </c>
-      <c r="P7" s="2">
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>5</v>
+      </c>
+      <c r="N7" s="3">
+        <v>5</v>
+      </c>
+      <c r="O7" s="3">
+        <v>5</v>
+      </c>
+      <c r="P7" s="3">
         <v>5</v>
       </c>
       <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="S7" s="9">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4">
-        <v>5</v>
-      </c>
-      <c r="M8" s="4">
+      <c r="C8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="M8" s="3">
         <v>5</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="S8" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="T8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4">
-        <v>5</v>
-      </c>
-      <c r="F9" s="5">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="M9" s="4">
-        <v>5</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="M9" s="3">
+        <v>5</v>
+      </c>
+      <c r="N9" s="3">
         <v>5</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="S9" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2"/>
@@ -810,46 +875,60 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="S10" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-      <c r="F11" s="5">
-        <v>5</v>
-      </c>
-      <c r="G11" s="5">
-        <v>5</v>
-      </c>
-      <c r="M11" s="4">
-        <v>5</v>
-      </c>
-      <c r="N11" s="4">
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5</v>
+      </c>
+      <c r="M11" s="3">
+        <v>5</v>
+      </c>
+      <c r="N11" s="3">
         <v>3</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="S11" s="9">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="2"/>
@@ -858,9 +937,16 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="S12" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -870,27 +956,34 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4">
-        <v>5</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
         <v>3</v>
       </c>
-      <c r="G13" s="7">
-        <v>5</v>
-      </c>
-      <c r="M13" s="2">
-        <v>5</v>
-      </c>
-      <c r="N13" s="4">
+      <c r="G13" s="6">
+        <v>5</v>
+      </c>
+      <c r="M13" s="3">
+        <v>5</v>
+      </c>
+      <c r="N13" s="3">
         <v>5</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="S13" s="9">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -906,9 +999,16 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="S14" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -924,9 +1024,16 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="S15" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -937,16 +1044,23 @@
         <v>13</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="M16" s="4">
+      <c r="M16" s="3">
         <v>5</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="S16" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -956,34 +1070,41 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="4">
-        <v>5</v>
-      </c>
-      <c r="E17" s="7">
-        <v>5</v>
-      </c>
-      <c r="G17" s="7">
-        <v>5</v>
-      </c>
-      <c r="H17" s="5">
-        <v>5</v>
-      </c>
-      <c r="M17" s="4">
-        <v>5</v>
-      </c>
-      <c r="N17" s="4">
-        <v>5</v>
-      </c>
-      <c r="O17" s="4">
-        <v>5</v>
-      </c>
-      <c r="P17" s="4">
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6">
+        <v>5</v>
+      </c>
+      <c r="G17" s="6">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5</v>
+      </c>
+      <c r="M17" s="3">
+        <v>5</v>
+      </c>
+      <c r="N17" s="3">
+        <v>5</v>
+      </c>
+      <c r="O17" s="3">
+        <v>5</v>
+      </c>
+      <c r="P17" s="3">
         <v>5</v>
       </c>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="S17" s="9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -993,19 +1114,26 @@
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="4">
-        <v>5</v>
-      </c>
-      <c r="M18" s="4">
+      <c r="D18" s="3">
+        <v>5</v>
+      </c>
+      <c r="M18" s="3">
         <v>5</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="S18" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="T18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1021,9 +1149,16 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="S19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1033,26 +1168,33 @@
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4">
-        <v>5</v>
-      </c>
-      <c r="G20" s="5">
-        <v>5</v>
-      </c>
-      <c r="M20" s="4">
-        <v>5</v>
-      </c>
-      <c r="N20" s="4">
+      <c r="D20" s="3">
+        <v>5</v>
+      </c>
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="M20" s="3">
+        <v>5</v>
+      </c>
+      <c r="N20" s="3">
         <v>5</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-      <c r="Q20" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="Q20" s="3">
+        <v>4</v>
+      </c>
+      <c r="S20" s="9">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="T20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1062,7 +1204,7 @@
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>5</v>
       </c>
       <c r="M21" s="2"/>
@@ -1070,9 +1212,16 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="S21" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1082,19 +1231,26 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="4">
-        <v>5</v>
-      </c>
-      <c r="M22" s="4">
+      <c r="D22" s="3">
+        <v>5</v>
+      </c>
+      <c r="M22" s="3">
         <v>5</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="S22" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="T22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1105,27 +1261,34 @@
         <v>20</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="G23">
-        <v>5</v>
-      </c>
-      <c r="H23">
-        <v>5</v>
-      </c>
-      <c r="M23" s="2">
-        <v>5</v>
-      </c>
-      <c r="N23" s="2">
+      <c r="F23" s="4">
+        <v>5</v>
+      </c>
+      <c r="G23" s="4">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+      <c r="M23" s="3">
+        <v>5</v>
+      </c>
+      <c r="N23" s="3">
         <v>5</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="S23" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="T23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -1136,24 +1299,31 @@
         <v>21</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="G24" s="5">
-        <v>5</v>
-      </c>
-      <c r="H24" s="5">
-        <v>5</v>
-      </c>
-      <c r="M24" s="4">
-        <v>5</v>
-      </c>
-      <c r="N24" s="4">
+      <c r="G24" s="4">
+        <v>5</v>
+      </c>
+      <c r="H24" s="4">
+        <v>5</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5</v>
+      </c>
+      <c r="N24" s="3">
         <v>4</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="S24" s="9">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="T24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -1169,9 +1339,16 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="S25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -1181,15 +1358,22 @@
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="3"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
+      <c r="S26" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1199,21 +1383,31 @@
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="4">
-        <v>5</v>
-      </c>
-      <c r="M27" s="4">
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
+        <v>4</v>
+      </c>
+      <c r="M27" s="3">
         <v>5</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
-      <c r="Q27" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
+      <c r="Q27" s="3">
+        <v>4</v>
+      </c>
+      <c r="S27" s="9">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="T27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -1223,29 +1417,274 @@
       <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="4">
-        <v>5</v>
+      <c r="D28" s="3">
+        <v>5</v>
+      </c>
+      <c r="H28" s="4">
+        <v>4</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
-      <c r="Q28" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="Q28" s="3">
+        <v>4</v>
+      </c>
+      <c r="S28" s="9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="T28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="3">
+        <v>4</v>
+      </c>
+      <c r="S29" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>5</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="3">
+        <v>4</v>
+      </c>
+      <c r="S30" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="3">
+        <v>5</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="3">
+        <v>4</v>
+      </c>
+      <c r="S31" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="3">
+        <v>5</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="3">
+        <v>4</v>
+      </c>
+      <c r="S32" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="3">
+        <v>5</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="3">
+        <v>4</v>
+      </c>
+      <c r="S33" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="3">
+        <v>5</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="3">
+        <v>4</v>
+      </c>
+      <c r="S34" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="3">
+        <v>4</v>
+      </c>
+      <c r="S35" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="3">
+        <v>5</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="3">
+        <v>4</v>
+      </c>
+      <c r="S36" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="3">
+        <v>5</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="3">
+        <v>4</v>
+      </c>
+      <c r="S37" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="T4:T28">
+  <conditionalFormatting sqref="S3:S37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>